<commit_message>
fix: Use openpyxl for xlsx reading and move to latest xlrd version
Create a set of excel utils to be used for .xls and .xlsx files, for
reading workbook, reading sheets, ... optimize openpyxl access to
sheet to save computation time.

Use this opportunity to refactor service sheet without namedtuple
and simplify code

Signed-off-by: EstherLerouzic <esther.lerouzic@orange.com>
Change-Id: Ibaf3aac40b3f6ca4829d8ea8cd506523d318103a
</commit_message>
<xml_diff>
--- a/tests/data/ila_constraint.xlsx
+++ b/tests/data/ila_constraint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\partage_vm\jeuTestWebapi\request-run\pierreLucOinisTrial400G\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\workspace\TIP\test\oopt-gnpy\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{75B67A3D-1BEB-47FA-8C1B-F0EE02649025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089541AC-2A09-4457-B89D-847C14CB840F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,14 @@
     <sheet name="Eqpt" sheetId="3" r:id="rId3"/>
     <sheet name="Service" sheetId="28" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="76">
   <si>
     <t>City</t>
   </si>
@@ -55,9 +57,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Dummy</t>
   </si>
   <si>
     <t>France</t>
@@ -292,7 +291,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -978,12 +977,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A4:Q184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,7 +1000,7 @@
   <sheetData>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1027,24 +1026,24 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
         <v>54</v>
-      </c>
-      <c r="I5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E6" s="27">
         <v>1</v>
@@ -1053,39 +1052,29 @@
         <v>0</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="27"/>
       <c r="L6" s="27"/>
-      <c r="M6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="27">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="27">
-        <v>0</v>
-      </c>
+      <c r="M6" s="22"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E7" s="27">
         <v>1.01</v>
@@ -1094,39 +1083,29 @@
         <v>0.01</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
-      <c r="M7" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" s="27">
-        <v>1.01</v>
-      </c>
-      <c r="Q7" s="27">
-        <v>0.01</v>
-      </c>
+      <c r="M7" s="22"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E8" s="27">
         <v>1.24</v>
@@ -1135,36 +1114,26 @@
         <v>0.24</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="27">
-        <v>1.02</v>
-      </c>
-      <c r="Q8" s="27">
-        <v>0.02</v>
-      </c>
+      <c r="M8" s="22"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E9" s="27">
         <v>1.25</v>
@@ -1173,21 +1142,21 @@
         <v>0.25</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E10" s="27">
         <v>1.25</v>
@@ -1196,21 +1165,21 @@
         <v>0.25</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E11" s="27">
         <v>1.25</v>
@@ -1219,21 +1188,21 @@
         <v>0.25</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E12" s="27">
         <v>1.25</v>
@@ -1242,21 +1211,21 @@
         <v>0.25</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>9</v>
       </c>
       <c r="E13" s="27">
         <v>1.25</v>
@@ -1265,7 +1234,7 @@
         <v>0.25</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1274,7 +1243,6 @@
       <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="G15" s="21"/>
     </row>
@@ -1311,6 +1279,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
       <c r="G22" s="21"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2114,14 +2083,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2147,27 +2116,27 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="4"/>
@@ -2176,7 +2145,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -2187,152 +2156,152 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="D5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="J5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2">
         <v>58.838999999999999</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3">
         <v>0.24</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2">
         <v>130</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3">
         <v>0.24</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2">
         <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="3">
         <v>0.24</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2">
         <v>54.341999999999999</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3">
         <v>0.24</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" s="3"/>
@@ -2341,10 +2310,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>64</v>
       </c>
       <c r="C11" s="2"/>
       <c r="E11" s="3"/>
@@ -2353,10 +2322,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2"/>
       <c r="E12" s="3"/>
@@ -2365,10 +2334,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2"/>
       <c r="E13" s="3"/>
@@ -2377,10 +2346,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2"/>
       <c r="E14" s="3"/>
@@ -2389,10 +2358,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2"/>
       <c r="E15" s="3"/>
@@ -2401,10 +2370,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>66</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>67</v>
       </c>
       <c r="C16" s="2"/>
       <c r="E16" s="3"/>
@@ -2652,11 +2621,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2675,24 +2644,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -2701,64 +2670,64 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>32</v>
-      </c>
       <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="L5" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2773,10 +2742,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A4:FB20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AI29" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -2802,65 +2771,65 @@
   <sheetData>
     <row r="4" spans="1:158" x14ac:dyDescent="0.3">
       <c r="I4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="K4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:158" s="20" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="C5" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="E5" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="F5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="G5" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="H5" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="I5" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="J5" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="K5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:158" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43">
@@ -2870,10 +2839,10 @@
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
       <c r="J6" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K6" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="43">
         <v>100</v>
@@ -2884,16 +2853,16 @@
     </row>
     <row r="7" spans="1:158" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="D7" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="43"/>
       <c r="F7" s="43">
@@ -2903,10 +2872,10 @@
       <c r="H7" s="43"/>
       <c r="I7" s="43"/>
       <c r="J7" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K7" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L7" s="43">
         <v>100</v>
@@ -2921,13 +2890,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="D8" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43">
@@ -2937,7 +2906,7 @@
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
       <c r="J8" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L8" s="43">
         <v>100</v>
@@ -2949,13 +2918,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="D9" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="43"/>
       <c r="F9" s="43">
@@ -2965,7 +2934,7 @@
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
       <c r="J9" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L9" s="43">
         <v>100</v>
@@ -2977,13 +2946,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="D10" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="43"/>
       <c r="F10" s="43">
@@ -2993,7 +2962,7 @@
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
       <c r="J10" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L10" s="43">
         <v>100</v>

</xml_diff>